<commit_message>
parse sharedStrings with font attributes
</commit_message>
<xml_diff>
--- a/src/Example Spreadsheet.xlsx
+++ b/src/Example Spreadsheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,20 +19,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Hello Excel</t>
+  </si>
+  <si>
+    <t>Hello Excel with the same color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hello </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Excel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>colors</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -57,14 +129,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -76,7 +217,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="ABE9A9"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -389,22 +530,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="29.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>